<commit_message>
ajuste na interacao com usuario
</commit_message>
<xml_diff>
--- a/automatizacao-planilhas-app-1/output/export_folha_de_pagamento_31072023.xlsx
+++ b/automatizacao-planilhas-app-1/output/export_folha_de_pagamento_31072023.xlsx
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>3509.812857142857</v>
+        <v>24568.69</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -542,7 +542,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>0.5014285714285714</v>
+        <v>3.51</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>155.3457142857143</v>
+        <v>1087.42</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -622,7 +622,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>51.78285714285715</v>
+        <v>362.48</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -662,7 +662,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>2.614285714285714</v>
+        <v>18.3</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>0.2828571428571429</v>
+        <v>1.98</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -742,7 +742,7 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>332.1271428571429</v>
+        <v>2324.89</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -782,7 +782,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>16.52</v>
+        <v>115.64</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -822,7 +822,7 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>1340.744285714286</v>
+        <v>9385.209999999999</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -862,7 +862,7 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>0.3942857142857143</v>
+        <v>2.76</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -902,7 +902,7 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>190.6085714285714</v>
+        <v>1334.26</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -942,7 +942,7 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>23.4</v>
+        <v>163.8</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -982,7 +982,7 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>51.72000000000001</v>
+        <v>362.04</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -1022,7 +1022,7 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>12.43428571428571</v>
+        <v>87.03999999999999</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -1062,7 +1062,7 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>20.8</v>
+        <v>145.6</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -1102,7 +1102,7 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>51.89714285714285</v>
+        <v>363.28</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1142,7 +1142,7 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1182,7 +1182,7 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>41.91714285714286</v>
+        <v>293.42</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1222,7 +1222,7 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>24.20571428571429</v>
+        <v>169.44</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1262,7 +1262,7 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>280.9557142857143</v>
+        <v>1966.69</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1302,7 +1302,7 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>638.0428571428572</v>
+        <v>4466.3</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1342,7 +1342,7 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>0.09571428571428572</v>
+        <v>0.67</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1382,7 +1382,7 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>64.45571428571428</v>
+        <v>451.19</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1422,7 +1422,7 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>255.2871428571429</v>
+        <v>1787.01</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1462,7 +1462,7 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>0.05285714285714286</v>
+        <v>0.37</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1502,7 +1502,7 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>3.342857142857143</v>
+        <v>23.4</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1542,7 +1542,7 @@
         </is>
       </c>
       <c r="F28" t="n">
-        <v>0.4285714285714285</v>
+        <v>3</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -1582,7 +1582,7 @@
         </is>
       </c>
       <c r="F29" t="n">
-        <v>51.04285714285714</v>
+        <v>357.3</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -1622,7 +1622,7 @@
         </is>
       </c>
       <c r="F30" t="n">
-        <v>674.0328571428571</v>
+        <v>4718.23</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -1662,7 +1662,7 @@
         </is>
       </c>
       <c r="F31" t="n">
-        <v>1.572857142857143</v>
+        <v>11.01</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -1702,7 +1702,7 @@
         </is>
       </c>
       <c r="F32" t="n">
-        <v>37.71428571428572</v>
+        <v>264</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -1742,7 +1742,7 @@
         </is>
       </c>
       <c r="F33" t="n">
-        <v>8.177142857142858</v>
+        <v>57.24</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -1782,7 +1782,7 @@
         </is>
       </c>
       <c r="F34" t="n">
-        <v>0.09428571428571429</v>
+        <v>0.66</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
@@ -1822,7 +1822,7 @@
         </is>
       </c>
       <c r="F35" t="n">
-        <v>76.13857142857144</v>
+        <v>532.97</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -1862,7 +1862,7 @@
         </is>
       </c>
       <c r="F36" t="n">
-        <v>269.6942857142857</v>
+        <v>1887.86</v>
       </c>
       <c r="G36" t="inlineStr">
         <is>
@@ -1902,7 +1902,7 @@
         </is>
       </c>
       <c r="F37" t="n">
-        <v>0.1071428571428571</v>
+        <v>0.75</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
@@ -1942,7 +1942,7 @@
         </is>
       </c>
       <c r="F38" t="n">
-        <v>3.342857142857143</v>
+        <v>23.4</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
@@ -1982,7 +1982,7 @@
         </is>
       </c>
       <c r="F39" t="n">
-        <v>12.93</v>
+        <v>90.51000000000001</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
@@ -2022,7 +2022,7 @@
         </is>
       </c>
       <c r="F40" t="n">
-        <v>0.4285714285714285</v>
+        <v>3</v>
       </c>
       <c r="G40" t="inlineStr">
         <is>
@@ -2062,7 +2062,7 @@
         </is>
       </c>
       <c r="F41" t="n">
-        <v>3.521428571428571</v>
+        <v>24.65</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
@@ -2102,7 +2102,7 @@
         </is>
       </c>
       <c r="F42" t="n">
-        <v>57.71857142857142</v>
+        <v>404.03</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -2142,7 +2142,7 @@
         </is>
       </c>
       <c r="F43" t="n">
-        <v>14800.85142857143</v>
+        <v>103605.96</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
@@ -2182,7 +2182,7 @@
         </is>
       </c>
       <c r="F44" t="n">
-        <v>54.37857142857143</v>
+        <v>380.65</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
@@ -2222,7 +2222,7 @@
         </is>
       </c>
       <c r="F45" t="n">
-        <v>501.4742857142857</v>
+        <v>3510.32</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -2262,7 +2262,7 @@
         </is>
       </c>
       <c r="F46" t="n">
-        <v>456.9857142857143</v>
+        <v>3198.9</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -2302,7 +2302,7 @@
         </is>
       </c>
       <c r="F47" t="n">
-        <v>1074.691428571429</v>
+        <v>7522.84</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -2342,7 +2342,7 @@
         </is>
       </c>
       <c r="F48" t="n">
-        <v>170.0228571428572</v>
+        <v>1190.16</v>
       </c>
       <c r="G48" t="inlineStr">
         <is>
@@ -2382,7 +2382,7 @@
         </is>
       </c>
       <c r="F49" t="n">
-        <v>358.23</v>
+        <v>2507.61</v>
       </c>
       <c r="G49" t="inlineStr">
         <is>
@@ -2422,7 +2422,7 @@
         </is>
       </c>
       <c r="F50" t="n">
-        <v>56.67428571428572</v>
+        <v>396.72</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
@@ -2462,7 +2462,7 @@
         </is>
       </c>
       <c r="F51" t="n">
-        <v>7.845714285714286</v>
+        <v>54.92</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
@@ -2502,7 +2502,7 @@
         </is>
       </c>
       <c r="F52" t="n">
-        <v>274.92</v>
+        <v>1924.44</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
@@ -2542,7 +2542,7 @@
         </is>
       </c>
       <c r="F53" t="n">
-        <v>171.1914285714286</v>
+        <v>1198.34</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
@@ -2582,7 +2582,7 @@
         </is>
       </c>
       <c r="F54" t="n">
-        <v>1.911428571428571</v>
+        <v>13.38</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
@@ -2622,7 +2622,7 @@
         </is>
       </c>
       <c r="F55" t="n">
-        <v>1568.475714285714</v>
+        <v>10979.33</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
@@ -2662,7 +2662,7 @@
         </is>
       </c>
       <c r="F56" t="n">
-        <v>150.0385714285714</v>
+        <v>1050.27</v>
       </c>
       <c r="G56" t="inlineStr">
         <is>
@@ -2702,7 +2702,7 @@
         </is>
       </c>
       <c r="F57" t="n">
-        <v>5810.551428571429</v>
+        <v>40673.86</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
@@ -2742,7 +2742,7 @@
         </is>
       </c>
       <c r="F58" t="n">
-        <v>1.755714285714286</v>
+        <v>12.29</v>
       </c>
       <c r="G58" t="inlineStr">
         <is>
@@ -2782,7 +2782,7 @@
         </is>
       </c>
       <c r="F59" t="n">
-        <v>1189.771428571428</v>
+        <v>8328.4</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
@@ -2822,7 +2822,7 @@
         </is>
       </c>
       <c r="F60" t="n">
-        <v>226.6971428571429</v>
+        <v>1586.88</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
@@ -2862,7 +2862,7 @@
         </is>
       </c>
       <c r="F61" t="n">
-        <v>86.91428571428571</v>
+        <v>608.4</v>
       </c>
       <c r="G61" t="inlineStr">
         <is>
@@ -2902,7 +2902,7 @@
         </is>
       </c>
       <c r="F62" t="n">
-        <v>255.5214285714286</v>
+        <v>1788.65</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
@@ -2942,7 +2942,7 @@
         </is>
       </c>
       <c r="F63" t="n">
-        <v>42.29285714285714</v>
+        <v>296.05</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
@@ -2982,7 +2982,7 @@
         </is>
       </c>
       <c r="F64" t="n">
-        <v>57.04285714285714</v>
+        <v>399.3</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
@@ -3022,7 +3022,7 @@
         </is>
       </c>
       <c r="F65" t="n">
-        <v>47.97142857142858</v>
+        <v>335.8</v>
       </c>
       <c r="G65" t="inlineStr">
         <is>
@@ -3062,7 +3062,7 @@
         </is>
       </c>
       <c r="F66" t="n">
-        <v>171.1914285714286</v>
+        <v>1198.34</v>
       </c>
       <c r="G66" t="inlineStr">
         <is>
@@ -3102,7 +3102,7 @@
         </is>
       </c>
       <c r="F67" t="n">
-        <v>192.1814285714286</v>
+        <v>1345.27</v>
       </c>
       <c r="G67" t="inlineStr">
         <is>
@@ -3142,7 +3142,7 @@
         </is>
       </c>
       <c r="F68" t="n">
-        <v>6.857142857142857</v>
+        <v>48</v>
       </c>
       <c r="G68" t="inlineStr">
         <is>
@@ -3182,7 +3182,7 @@
         </is>
       </c>
       <c r="F69" t="n">
-        <v>157.1428571428571</v>
+        <v>1100</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
@@ -3222,7 +3222,7 @@
         </is>
       </c>
       <c r="F70" t="n">
-        <v>11.14285714285714</v>
+        <v>78</v>
       </c>
       <c r="G70" t="inlineStr">
         <is>
@@ -3262,7 +3262,7 @@
         </is>
       </c>
       <c r="F71" t="n">
-        <v>116.1128571428571</v>
+        <v>812.79</v>
       </c>
       <c r="G71" t="inlineStr">
         <is>
@@ -3302,7 +3302,7 @@
         </is>
       </c>
       <c r="F72" t="n">
-        <v>129.0671428571429</v>
+        <v>903.47</v>
       </c>
       <c r="G72" t="inlineStr">
         <is>
@@ -3342,7 +3342,7 @@
         </is>
       </c>
       <c r="F73" t="n">
-        <v>242.0514285714286</v>
+        <v>1694.36</v>
       </c>
       <c r="G73" t="inlineStr">
         <is>
@@ -3382,7 +3382,7 @@
         </is>
       </c>
       <c r="F74" t="n">
-        <v>93.11142857142858</v>
+        <v>651.7800000000001</v>
       </c>
       <c r="G74" t="inlineStr">
         <is>
@@ -3422,7 +3422,7 @@
         </is>
       </c>
       <c r="F75" t="n">
-        <v>1432.921428571429</v>
+        <v>10030.45</v>
       </c>
       <c r="G75" t="inlineStr">
         <is>
@@ -3462,7 +3462,7 @@
         </is>
       </c>
       <c r="F76" t="n">
-        <v>890.8542857142857</v>
+        <v>6235.98</v>
       </c>
       <c r="G76" t="inlineStr">
         <is>
@@ -3502,7 +3502,7 @@
         </is>
       </c>
       <c r="F77" t="n">
-        <v>28.87571428571428</v>
+        <v>202.13</v>
       </c>
       <c r="G77" t="inlineStr">
         <is>
@@ -3542,7 +3542,7 @@
         </is>
       </c>
       <c r="F78" t="n">
-        <v>267.17</v>
+        <v>1870.19</v>
       </c>
       <c r="G78" t="inlineStr">
         <is>
@@ -3582,7 +3582,7 @@
         </is>
       </c>
       <c r="F79" t="n">
-        <v>147.7971428571429</v>
+        <v>1034.58</v>
       </c>
       <c r="G79" t="inlineStr">
         <is>
@@ -3622,7 +3622,7 @@
         </is>
       </c>
       <c r="F80" t="n">
-        <v>2.354285714285715</v>
+        <v>16.48</v>
       </c>
       <c r="G80" t="inlineStr">
         <is>
@@ -3662,7 +3662,7 @@
         </is>
       </c>
       <c r="F81" t="n">
-        <v>0.2628571428571429</v>
+        <v>1.84</v>
       </c>
       <c r="G81" t="inlineStr">
         <is>
@@ -3702,7 +3702,7 @@
         </is>
       </c>
       <c r="F82" t="n">
-        <v>137.87</v>
+        <v>965.09</v>
       </c>
       <c r="G82" t="inlineStr">
         <is>
@@ -3742,7 +3742,7 @@
         </is>
       </c>
       <c r="F83" t="n">
-        <v>356.3857142857143</v>
+        <v>2494.7</v>
       </c>
       <c r="G83" t="inlineStr">
         <is>
@@ -3782,7 +3782,7 @@
         </is>
       </c>
       <c r="F84" t="n">
-        <v>0.1057142857142857</v>
+        <v>0.74</v>
       </c>
       <c r="G84" t="inlineStr">
         <is>
@@ -3822,7 +3822,7 @@
         </is>
       </c>
       <c r="F85" t="n">
-        <v>6.685714285714285</v>
+        <v>46.8</v>
       </c>
       <c r="G85" t="inlineStr">
         <is>
@@ -3862,7 +3862,7 @@
         </is>
       </c>
       <c r="F86" t="n">
-        <v>0.2871428571428571</v>
+        <v>2.01</v>
       </c>
       <c r="G86" t="inlineStr">
         <is>
@@ -3902,7 +3902,7 @@
         </is>
       </c>
       <c r="F87" t="n">
-        <v>3.46</v>
+        <v>24.22</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
@@ -3942,7 +3942,7 @@
         </is>
       </c>
       <c r="F88" t="n">
-        <v>142.8571428571429</v>
+        <v>1000</v>
       </c>
       <c r="G88" t="inlineStr">
         <is>
@@ -3982,7 +3982,7 @@
         </is>
       </c>
       <c r="F89" t="n">
-        <v>0.8571428571428571</v>
+        <v>6</v>
       </c>
       <c r="G89" t="inlineStr">
         <is>
@@ -4022,7 +4022,7 @@
         </is>
       </c>
       <c r="F90" t="n">
-        <v>23.66285714285714</v>
+        <v>165.64</v>
       </c>
       <c r="G90" t="inlineStr">
         <is>
@@ -4062,7 +4062,7 @@
         </is>
       </c>
       <c r="F91" t="n">
-        <v>22.85714285714286</v>
+        <v>160</v>
       </c>
       <c r="G91" t="inlineStr">
         <is>
@@ -4102,7 +4102,7 @@
         </is>
       </c>
       <c r="F92" t="n">
-        <v>106.9385714285714</v>
+        <v>748.5699999999999</v>
       </c>
       <c r="G92" t="inlineStr">
         <is>
@@ -4142,7 +4142,7 @@
         </is>
       </c>
       <c r="F93" t="n">
-        <v>875.5914285714287</v>
+        <v>6129.14</v>
       </c>
       <c r="G93" t="inlineStr">
         <is>
@@ -4182,7 +4182,7 @@
         </is>
       </c>
       <c r="F94" t="n">
-        <v>7.422857142857143</v>
+        <v>51.96</v>
       </c>
       <c r="G94" t="inlineStr">
         <is>
@@ -4222,7 +4222,7 @@
         </is>
       </c>
       <c r="F95" t="n">
-        <v>29.51</v>
+        <v>206.57</v>
       </c>
       <c r="G95" t="inlineStr">
         <is>
@@ -4262,7 +4262,7 @@
         </is>
       </c>
       <c r="F96" t="n">
-        <v>9.091428571428573</v>
+        <v>63.64</v>
       </c>
       <c r="G96" t="inlineStr">
         <is>
@@ -4302,7 +4302,7 @@
         </is>
       </c>
       <c r="F97" t="n">
-        <v>0.1742857142857143</v>
+        <v>1.22</v>
       </c>
       <c r="G97" t="inlineStr">
         <is>
@@ -4342,7 +4342,7 @@
         </is>
       </c>
       <c r="F98" t="n">
-        <v>82.87571428571428</v>
+        <v>580.13</v>
       </c>
       <c r="G98" t="inlineStr">
         <is>
@@ -4382,7 +4382,7 @@
         </is>
       </c>
       <c r="F99" t="n">
-        <v>350.3971428571429</v>
+        <v>2452.78</v>
       </c>
       <c r="G99" t="inlineStr">
         <is>
@@ -4422,7 +4422,7 @@
         </is>
       </c>
       <c r="F100" t="n">
-        <v>0.04142857142857143</v>
+        <v>0.29</v>
       </c>
       <c r="G100" t="inlineStr">
         <is>
@@ -4462,7 +4462,7 @@
         </is>
       </c>
       <c r="F101" t="n">
-        <v>6.685714285714285</v>
+        <v>46.8</v>
       </c>
       <c r="G101" t="inlineStr">
         <is>
@@ -4502,7 +4502,7 @@
         </is>
       </c>
       <c r="F102" t="n">
-        <v>17.92857142857143</v>
+        <v>125.5</v>
       </c>
       <c r="G102" t="inlineStr">
         <is>
@@ -4542,7 +4542,7 @@
         </is>
       </c>
       <c r="F103" t="n">
-        <v>0.1471428571428571</v>
+        <v>1.03</v>
       </c>
       <c r="G103" t="inlineStr">
         <is>
@@ -4582,7 +4582,7 @@
         </is>
       </c>
       <c r="F104" t="n">
-        <v>0.8571428571428571</v>
+        <v>6</v>
       </c>
       <c r="G104" t="inlineStr">
         <is>
@@ -4622,7 +4622,7 @@
         </is>
       </c>
       <c r="F105" t="n">
-        <v>73.71571428571428</v>
+        <v>516.01</v>
       </c>
       <c r="G105" t="inlineStr">
         <is>
@@ -4662,7 +4662,7 @@
         </is>
       </c>
       <c r="F106" t="n">
-        <v>1549.087142857143</v>
+        <v>10843.61</v>
       </c>
       <c r="G106" t="inlineStr">
         <is>
@@ -4702,7 +4702,7 @@
         </is>
       </c>
       <c r="F107" t="n">
-        <v>103.3114285714286</v>
+        <v>723.1800000000001</v>
       </c>
       <c r="G107" t="inlineStr">
         <is>
@@ -4742,7 +4742,7 @@
         </is>
       </c>
       <c r="F108" t="n">
-        <v>141.1014285714286</v>
+        <v>987.71</v>
       </c>
       <c r="G108" t="inlineStr">
         <is>
@@ -4782,7 +4782,7 @@
         </is>
       </c>
       <c r="F109" t="n">
-        <v>468.9114285714285</v>
+        <v>3282.38</v>
       </c>
       <c r="G109" t="inlineStr">
         <is>
@@ -4822,7 +4822,7 @@
         </is>
       </c>
       <c r="F110" t="n">
-        <v>156.3028571428571</v>
+        <v>1094.12</v>
       </c>
       <c r="G110" t="inlineStr">
         <is>
@@ -4862,7 +4862,7 @@
         </is>
       </c>
       <c r="F111" t="n">
-        <v>124.8185714285714</v>
+        <v>873.73</v>
       </c>
       <c r="G111" t="inlineStr">
         <is>
@@ -4902,7 +4902,7 @@
         </is>
       </c>
       <c r="F112" t="n">
-        <v>262.6957142857142</v>
+        <v>1838.87</v>
       </c>
       <c r="G112" t="inlineStr">
         <is>
@@ -4942,7 +4942,7 @@
         </is>
       </c>
       <c r="F113" t="n">
-        <v>8.595714285714285</v>
+        <v>60.17</v>
       </c>
       <c r="G113" t="inlineStr">
         <is>
@@ -4982,7 +4982,7 @@
         </is>
       </c>
       <c r="F114" t="n">
-        <v>0.3028571428571428</v>
+        <v>2.12</v>
       </c>
       <c r="G114" t="inlineStr">
         <is>
@@ -5022,7 +5022,7 @@
         </is>
       </c>
       <c r="F115" t="n">
-        <v>222.3257142857143</v>
+        <v>1556.28</v>
       </c>
       <c r="G115" t="inlineStr">
         <is>
@@ -5062,7 +5062,7 @@
         </is>
       </c>
       <c r="F116" t="n">
-        <v>60.17285714285714</v>
+        <v>421.21</v>
       </c>
       <c r="G116" t="inlineStr">
         <is>
@@ -5102,7 +5102,7 @@
         </is>
       </c>
       <c r="F117" t="n">
-        <v>23.14285714285714</v>
+        <v>162</v>
       </c>
       <c r="G117" t="inlineStr">
         <is>
@@ -5142,7 +5142,7 @@
         </is>
       </c>
       <c r="F118" t="n">
-        <v>631.8071428571429</v>
+        <v>4422.65</v>
       </c>
       <c r="G118" t="inlineStr">
         <is>
@@ -5182,7 +5182,7 @@
         </is>
       </c>
       <c r="F119" t="n">
-        <v>0.3528571428571429</v>
+        <v>2.47</v>
       </c>
       <c r="G119" t="inlineStr">
         <is>
@@ -5222,7 +5222,7 @@
         </is>
       </c>
       <c r="F120" t="n">
-        <v>550.6185714285714</v>
+        <v>3854.33</v>
       </c>
       <c r="G120" t="inlineStr">
         <is>
@@ -5262,7 +5262,7 @@
         </is>
       </c>
       <c r="F121" t="n">
-        <v>5.248571428571428</v>
+        <v>36.74</v>
       </c>
       <c r="G121" t="inlineStr">
         <is>
@@ -5302,7 +5302,7 @@
         </is>
       </c>
       <c r="F122" t="n">
-        <v>1.192857142857143</v>
+        <v>8.35</v>
       </c>
       <c r="G122" t="inlineStr">
         <is>
@@ -5342,7 +5342,7 @@
         </is>
       </c>
       <c r="F123" t="n">
-        <v>58.19428571428572</v>
+        <v>407.36</v>
       </c>
       <c r="G123" t="inlineStr">
         <is>
@@ -5382,7 +5382,7 @@
         </is>
       </c>
       <c r="F124" t="n">
-        <v>2.142857142857143</v>
+        <v>15</v>
       </c>
       <c r="G124" t="inlineStr">
         <is>
@@ -5422,7 +5422,7 @@
         </is>
       </c>
       <c r="F125" t="n">
-        <v>64.07714285714286</v>
+        <v>448.54</v>
       </c>
       <c r="G125" t="inlineStr">
         <is>
@@ -5462,7 +5462,7 @@
         </is>
       </c>
       <c r="F126" t="n">
-        <v>14.42285714285714</v>
+        <v>100.96</v>
       </c>
       <c r="G126" t="inlineStr">
         <is>
@@ -5502,7 +5502,7 @@
         </is>
       </c>
       <c r="F127" t="n">
-        <v>224.7614285714286</v>
+        <v>1573.33</v>
       </c>
       <c r="G127" t="inlineStr">
         <is>
@@ -5542,7 +5542,7 @@
         </is>
       </c>
       <c r="F128" t="n">
-        <v>1786.547142857143</v>
+        <v>12505.83</v>
       </c>
       <c r="G128" t="inlineStr">
         <is>
@@ -5582,7 +5582,7 @@
         </is>
       </c>
       <c r="F129" t="n">
-        <v>58.92857142857143</v>
+        <v>412.5</v>
       </c>
       <c r="G129" t="inlineStr">
         <is>
@@ -5622,7 +5622,7 @@
         </is>
       </c>
       <c r="F130" t="n">
-        <v>139.8885714285714</v>
+        <v>979.22</v>
       </c>
       <c r="G130" t="inlineStr">
         <is>
@@ -5662,7 +5662,7 @@
         </is>
       </c>
       <c r="F131" t="n">
-        <v>74.05142857142857</v>
+        <v>518.36</v>
       </c>
       <c r="G131" t="inlineStr">
         <is>
@@ -5702,7 +5702,7 @@
         </is>
       </c>
       <c r="F132" t="n">
-        <v>40.81857142857143</v>
+        <v>285.73</v>
       </c>
       <c r="G132" t="inlineStr">
         <is>
@@ -5742,7 +5742,7 @@
         </is>
       </c>
       <c r="F133" t="n">
-        <v>50.92142857142858</v>
+        <v>356.45</v>
       </c>
       <c r="G133" t="inlineStr">
         <is>
@@ -5782,7 +5782,7 @@
         </is>
       </c>
       <c r="F134" t="n">
-        <v>0.3057142857142857</v>
+        <v>2.14</v>
       </c>
       <c r="G134" t="inlineStr">
         <is>
@@ -5822,7 +5822,7 @@
         </is>
       </c>
       <c r="F135" t="n">
-        <v>199.8214285714286</v>
+        <v>1398.75</v>
       </c>
       <c r="G135" t="inlineStr">
         <is>
@@ -5862,7 +5862,7 @@
         </is>
       </c>
       <c r="F136" t="n">
-        <v>658.7085714285714</v>
+        <v>4610.96</v>
       </c>
       <c r="G136" t="inlineStr">
         <is>
@@ -5902,7 +5902,7 @@
         </is>
       </c>
       <c r="F137" t="n">
-        <v>0.3371428571428571</v>
+        <v>2.36</v>
       </c>
       <c r="G137" t="inlineStr">
         <is>
@@ -5942,7 +5942,7 @@
         </is>
       </c>
       <c r="F138" t="n">
-        <v>16.71428571428571</v>
+        <v>117</v>
       </c>
       <c r="G138" t="inlineStr">
         <is>
@@ -5982,7 +5982,7 @@
         </is>
       </c>
       <c r="F139" t="n">
-        <v>77.85714285714286</v>
+        <v>545</v>
       </c>
       <c r="G139" t="inlineStr">
         <is>
@@ -6022,7 +6022,7 @@
         </is>
       </c>
       <c r="F140" t="n">
-        <v>4.941428571428571</v>
+        <v>34.59</v>
       </c>
       <c r="G140" t="inlineStr">
         <is>
@@ -6062,7 +6062,7 @@
         </is>
       </c>
       <c r="F141" t="n">
-        <v>9.347142857142858</v>
+        <v>65.43000000000001</v>
       </c>
       <c r="G141" t="inlineStr">
         <is>
@@ -6102,7 +6102,7 @@
         </is>
       </c>
       <c r="F142" t="n">
-        <v>2.142857142857143</v>
+        <v>15</v>
       </c>
       <c r="G142" t="inlineStr">
         <is>
@@ -6142,7 +6142,7 @@
         </is>
       </c>
       <c r="F143" t="n">
-        <v>9.305714285714286</v>
+        <v>65.13999999999999</v>
       </c>
       <c r="G143" t="inlineStr">
         <is>
@@ -6182,7 +6182,7 @@
         </is>
       </c>
       <c r="F144" t="n">
-        <v>170.9457142857143</v>
+        <v>1196.62</v>
       </c>
       <c r="G144" t="inlineStr">
         <is>
@@ -6222,7 +6222,7 @@
         </is>
       </c>
       <c r="F145" t="n">
-        <v>579.52</v>
+        <v>4056.64</v>
       </c>
       <c r="G145" t="inlineStr">
         <is>
@@ -6262,7 +6262,7 @@
         </is>
       </c>
       <c r="F146" t="n">
-        <v>12.54</v>
+        <v>87.78</v>
       </c>
       <c r="G146" t="inlineStr">
         <is>
@@ -6302,7 +6302,7 @@
         </is>
       </c>
       <c r="F147" t="n">
-        <v>33.48142857142857</v>
+        <v>234.37</v>
       </c>
       <c r="G147" t="inlineStr">
         <is>
@@ -6342,7 +6342,7 @@
         </is>
       </c>
       <c r="F148" t="n">
-        <v>6.27</v>
+        <v>43.89</v>
       </c>
       <c r="G148" t="inlineStr">
         <is>
@@ -6382,7 +6382,7 @@
         </is>
       </c>
       <c r="F149" t="n">
-        <v>25.45714285714286</v>
+        <v>178.2</v>
       </c>
       <c r="G149" t="inlineStr">
         <is>
@@ -6422,7 +6422,7 @@
         </is>
       </c>
       <c r="F150" t="n">
-        <v>0.04285714285714286</v>
+        <v>0.3</v>
       </c>
       <c r="G150" t="inlineStr">
         <is>
@@ -6462,7 +6462,7 @@
         </is>
       </c>
       <c r="F151" t="n">
-        <v>53.45428571428572</v>
+        <v>374.1799999999999</v>
       </c>
       <c r="G151" t="inlineStr">
         <is>
@@ -6502,7 +6502,7 @@
         </is>
       </c>
       <c r="F152" t="n">
-        <v>8.4</v>
+        <v>58.8</v>
       </c>
       <c r="G152" t="inlineStr">
         <is>
@@ -6542,7 +6542,7 @@
         </is>
       </c>
       <c r="F153" t="n">
-        <v>232</v>
+        <v>1624</v>
       </c>
       <c r="G153" t="inlineStr">
         <is>
@@ -6582,7 +6582,7 @@
         </is>
       </c>
       <c r="F154" t="n">
-        <v>0.14</v>
+        <v>0.98</v>
       </c>
       <c r="G154" t="inlineStr">
         <is>
@@ -6622,7 +6622,7 @@
         </is>
       </c>
       <c r="F155" t="n">
-        <v>0.46</v>
+        <v>3.22</v>
       </c>
       <c r="G155" t="inlineStr">
         <is>
@@ -6662,7 +6662,7 @@
         </is>
       </c>
       <c r="F156" t="n">
-        <v>0.8571428571428571</v>
+        <v>6</v>
       </c>
       <c r="G156" t="inlineStr">
         <is>
@@ -6702,7 +6702,7 @@
         </is>
       </c>
       <c r="F157" t="n">
-        <v>52.54428571428571</v>
+        <v>367.81</v>
       </c>
       <c r="G157" t="inlineStr">
         <is>
@@ -6742,7 +6742,7 @@
         </is>
       </c>
       <c r="F158" t="n">
-        <v>616.2228571428572</v>
+        <v>4313.56</v>
       </c>
       <c r="G158" t="inlineStr">
         <is>
@@ -6782,7 +6782,7 @@
         </is>
       </c>
       <c r="F159" t="n">
-        <v>4.761428571428572</v>
+        <v>33.33</v>
       </c>
       <c r="G159" t="inlineStr">
         <is>
@@ -6822,7 +6822,7 @@
         </is>
       </c>
       <c r="F160" t="n">
-        <v>24.76142857142857</v>
+        <v>173.33</v>
       </c>
       <c r="G160" t="inlineStr">
         <is>
@@ -6862,7 +6862,7 @@
         </is>
       </c>
       <c r="F161" t="n">
-        <v>0.1371428571428571</v>
+        <v>0.9600000000000001</v>
       </c>
       <c r="G161" t="inlineStr">
         <is>
@@ -6902,7 +6902,7 @@
         </is>
       </c>
       <c r="F162" t="n">
-        <v>52.30142857142857</v>
+        <v>366.11</v>
       </c>
       <c r="G162" t="inlineStr">
         <is>
@@ -6942,7 +6942,7 @@
         </is>
       </c>
       <c r="F163" t="n">
-        <v>8.4</v>
+        <v>58.8</v>
       </c>
       <c r="G163" t="inlineStr">
         <is>
@@ -6982,7 +6982,7 @@
         </is>
       </c>
       <c r="F164" t="n">
-        <v>246.5714285714286</v>
+        <v>1726</v>
       </c>
       <c r="G164" t="inlineStr">
         <is>
@@ -7022,7 +7022,7 @@
         </is>
       </c>
       <c r="F165" t="n">
-        <v>0.2428571428571428</v>
+        <v>1.7</v>
       </c>
       <c r="G165" t="inlineStr">
         <is>
@@ -7062,7 +7062,7 @@
         </is>
       </c>
       <c r="F166" t="n">
-        <v>24</v>
+        <v>168</v>
       </c>
       <c r="G166" t="inlineStr">
         <is>
@@ -7102,7 +7102,7 @@
         </is>
       </c>
       <c r="F167" t="n">
-        <v>1.737142857142857</v>
+        <v>12.16</v>
       </c>
       <c r="G167" t="inlineStr">
         <is>
@@ -7142,7 +7142,7 @@
         </is>
       </c>
       <c r="F168" t="n">
-        <v>18.48714285714286</v>
+        <v>129.41</v>
       </c>
       <c r="G168" t="inlineStr">
         <is>
@@ -7182,7 +7182,7 @@
         </is>
       </c>
       <c r="F169" t="n">
-        <v>0.8571428571428571</v>
+        <v>6</v>
       </c>
       <c r="G169" t="inlineStr">
         <is>
@@ -7222,7 +7222,7 @@
         </is>
       </c>
       <c r="F170" t="n">
-        <v>51.51857142857143</v>
+        <v>360.63</v>
       </c>
       <c r="G170" t="inlineStr">
         <is>
@@ -7262,7 +7262,7 @@
         </is>
       </c>
       <c r="F171" t="n">
-        <v>933.4542857142857</v>
+        <v>6534.18</v>
       </c>
       <c r="G171" t="inlineStr">
         <is>
@@ -7302,7 +7302,7 @@
         </is>
       </c>
       <c r="F172" t="n">
-        <v>29.78</v>
+        <v>208.46</v>
       </c>
       <c r="G172" t="inlineStr">
         <is>
@@ -7342,7 +7342,7 @@
         </is>
       </c>
       <c r="F173" t="n">
-        <v>23.9</v>
+        <v>167.3</v>
       </c>
       <c r="G173" t="inlineStr">
         <is>
@@ -7382,7 +7382,7 @@
         </is>
       </c>
       <c r="F174" t="n">
-        <v>57.59714285714286</v>
+        <v>403.18</v>
       </c>
       <c r="G174" t="inlineStr">
         <is>
@@ -7422,7 +7422,7 @@
         </is>
       </c>
       <c r="F175" t="n">
-        <v>19.19857142857143</v>
+        <v>134.39</v>
       </c>
       <c r="G175" t="inlineStr">
         <is>
@@ -7462,7 +7462,7 @@
         </is>
       </c>
       <c r="F176" t="n">
-        <v>33.69571428571429</v>
+        <v>235.87</v>
       </c>
       <c r="G176" t="inlineStr">
         <is>
@@ -7502,7 +7502,7 @@
         </is>
       </c>
       <c r="F177" t="n">
-        <v>88.18571428571428</v>
+        <v>617.3000000000001</v>
       </c>
       <c r="G177" t="inlineStr">
         <is>
@@ -7542,7 +7542,7 @@
         </is>
       </c>
       <c r="F178" t="n">
-        <v>3.292857142857143</v>
+        <v>23.05</v>
       </c>
       <c r="G178" t="inlineStr">
         <is>
@@ -7582,7 +7582,7 @@
         </is>
       </c>
       <c r="F179" t="n">
-        <v>3.504285714285714</v>
+        <v>24.53</v>
       </c>
       <c r="G179" t="inlineStr">
         <is>
@@ -7622,7 +7622,7 @@
         </is>
       </c>
       <c r="F180" t="n">
-        <v>5.785714285714286</v>
+        <v>40.5</v>
       </c>
       <c r="G180" t="inlineStr">
         <is>
@@ -7662,7 +7662,7 @@
         </is>
       </c>
       <c r="F181" t="n">
-        <v>0.2471428571428571</v>
+        <v>1.73</v>
       </c>
       <c r="G181" t="inlineStr">
         <is>
@@ -7702,7 +7702,7 @@
         </is>
       </c>
       <c r="F182" t="n">
-        <v>93.48714285714286</v>
+        <v>654.41</v>
       </c>
       <c r="G182" t="inlineStr">
         <is>
@@ -7742,7 +7742,7 @@
         </is>
       </c>
       <c r="F183" t="n">
-        <v>7.435714285714285</v>
+        <v>52.05</v>
       </c>
       <c r="G183" t="inlineStr">
         <is>
@@ -7782,7 +7782,7 @@
         </is>
       </c>
       <c r="F184" t="n">
-        <v>12.6</v>
+        <v>88.19999999999999</v>
       </c>
       <c r="G184" t="inlineStr">
         <is>
@@ -7822,7 +7822,7 @@
         </is>
       </c>
       <c r="F185" t="n">
-        <v>393.4285714285714</v>
+        <v>2754</v>
       </c>
       <c r="G185" t="inlineStr">
         <is>
@@ -7862,7 +7862,7 @@
         </is>
       </c>
       <c r="F186" t="n">
-        <v>0.1871428571428572</v>
+        <v>1.31</v>
       </c>
       <c r="G186" t="inlineStr">
         <is>
@@ -7902,7 +7902,7 @@
         </is>
       </c>
       <c r="F187" t="n">
-        <v>52.95428571428572</v>
+        <v>370.68</v>
       </c>
       <c r="G187" t="inlineStr">
         <is>
@@ -7942,7 +7942,7 @@
         </is>
       </c>
       <c r="F188" t="n">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="G188" t="inlineStr">
         <is>
@@ -7982,7 +7982,7 @@
         </is>
       </c>
       <c r="F189" t="n">
-        <v>19.26428571428571</v>
+        <v>134.85</v>
       </c>
       <c r="G189" t="inlineStr">
         <is>
@@ -8022,7 +8022,7 @@
         </is>
       </c>
       <c r="F190" t="n">
-        <v>59.52428571428572</v>
+        <v>416.67</v>
       </c>
       <c r="G190" t="inlineStr">
         <is>
@@ -8062,7 +8062,7 @@
         </is>
       </c>
       <c r="F191" t="n">
-        <v>1.285714285714286</v>
+        <v>9</v>
       </c>
       <c r="G191" t="inlineStr">
         <is>
@@ -8102,7 +8102,7 @@
         </is>
       </c>
       <c r="F192" t="n">
-        <v>15.36</v>
+        <v>107.52</v>
       </c>
       <c r="G192" t="inlineStr">
         <is>
@@ -8142,7 +8142,7 @@
         </is>
       </c>
       <c r="F193" t="n">
-        <v>69.35428571428572</v>
+        <v>485.48</v>
       </c>
       <c r="G193" t="inlineStr">
         <is>
@@ -8182,7 +8182,7 @@
         </is>
       </c>
       <c r="F194" t="n">
-        <v>1.045714285714286</v>
+        <v>7.32</v>
       </c>
       <c r="G194" t="inlineStr">
         <is>
@@ -8222,7 +8222,7 @@
         </is>
       </c>
       <c r="F195" t="n">
-        <v>95.47</v>
+        <v>668.29</v>
       </c>
       <c r="G195" t="inlineStr">
         <is>
@@ -8262,7 +8262,7 @@
         </is>
       </c>
       <c r="F196" t="n">
-        <v>1239.802857142857</v>
+        <v>8678.620000000001</v>
       </c>
       <c r="G196" t="inlineStr">
         <is>
@@ -8302,7 +8302,7 @@
         </is>
       </c>
       <c r="F197" t="n">
-        <v>49.57857142857143</v>
+        <v>347.05</v>
       </c>
       <c r="G197" t="inlineStr">
         <is>
@@ -8342,7 +8342,7 @@
         </is>
       </c>
       <c r="F198" t="n">
-        <v>128.02</v>
+        <v>896.14</v>
       </c>
       <c r="G198" t="inlineStr">
         <is>
@@ -8382,7 +8382,7 @@
         </is>
       </c>
       <c r="F199" t="n">
-        <v>450.6271428571428</v>
+        <v>3154.39</v>
       </c>
       <c r="G199" t="inlineStr">
         <is>
@@ -8422,7 +8422,7 @@
         </is>
       </c>
       <c r="F200" t="n">
-        <v>45.06285714285714</v>
+        <v>315.44</v>
       </c>
       <c r="G200" t="inlineStr">
         <is>
@@ -8462,7 +8462,7 @@
         </is>
       </c>
       <c r="F201" t="n">
-        <v>150.2085714285714</v>
+        <v>1051.46</v>
       </c>
       <c r="G201" t="inlineStr">
         <is>
@@ -8502,7 +8502,7 @@
         </is>
       </c>
       <c r="F202" t="n">
-        <v>15.02142857142857</v>
+        <v>105.15</v>
       </c>
       <c r="G202" t="inlineStr">
         <is>
@@ -8542,7 +8542,7 @@
         </is>
       </c>
       <c r="F203" t="n">
-        <v>57.5</v>
+        <v>402.5</v>
       </c>
       <c r="G203" t="inlineStr">
         <is>
@@ -8582,7 +8582,7 @@
         </is>
       </c>
       <c r="F204" t="n">
-        <v>72.29285714285714</v>
+        <v>506.05</v>
       </c>
       <c r="G204" t="inlineStr">
         <is>
@@ -8622,7 +8622,7 @@
         </is>
       </c>
       <c r="F205" t="n">
-        <v>0.29</v>
+        <v>2.03</v>
       </c>
       <c r="G205" t="inlineStr">
         <is>
@@ -8662,7 +8662,7 @@
         </is>
       </c>
       <c r="F206" t="n">
-        <v>149.3442857142857</v>
+        <v>1045.41</v>
       </c>
       <c r="G206" t="inlineStr">
         <is>
@@ -8702,7 +8702,7 @@
         </is>
       </c>
       <c r="F207" t="n">
-        <v>59.24571428571429</v>
+        <v>414.72</v>
       </c>
       <c r="G207" t="inlineStr">
         <is>
@@ -8742,7 +8742,7 @@
         </is>
       </c>
       <c r="F208" t="n">
-        <v>10.45714285714286</v>
+        <v>73.19999999999999</v>
       </c>
       <c r="G208" t="inlineStr">
         <is>
@@ -8782,7 +8782,7 @@
         </is>
       </c>
       <c r="F209" t="n">
-        <v>393.4685714285714</v>
+        <v>2754.28</v>
       </c>
       <c r="G209" t="inlineStr">
         <is>
@@ -8822,7 +8822,7 @@
         </is>
       </c>
       <c r="F210" t="n">
-        <v>0.2971428571428572</v>
+        <v>2.08</v>
       </c>
       <c r="G210" t="inlineStr">
         <is>
@@ -8862,7 +8862,7 @@
         </is>
       </c>
       <c r="F211" t="n">
-        <v>517.3285714285714</v>
+        <v>3621.3</v>
       </c>
       <c r="G211" t="inlineStr">
         <is>
@@ -8902,7 +8902,7 @@
         </is>
       </c>
       <c r="F212" t="n">
-        <v>60.08428571428571</v>
+        <v>420.59</v>
       </c>
       <c r="G212" t="inlineStr">
         <is>
@@ -8942,7 +8942,7 @@
         </is>
       </c>
       <c r="F213" t="n">
-        <v>3.485714285714285</v>
+        <v>24.4</v>
       </c>
       <c r="G213" t="inlineStr">
         <is>
@@ -8982,7 +8982,7 @@
         </is>
       </c>
       <c r="F214" t="n">
-        <v>45.61142857142857</v>
+        <v>319.28</v>
       </c>
       <c r="G214" t="inlineStr">
         <is>
@@ -9022,7 +9022,7 @@
         </is>
       </c>
       <c r="F215" t="n">
-        <v>0.3157142857142857</v>
+        <v>2.21</v>
       </c>
       <c r="G215" t="inlineStr">
         <is>
@@ -9062,7 +9062,7 @@
         </is>
       </c>
       <c r="F216" t="n">
-        <v>134.92</v>
+        <v>944.4400000000001</v>
       </c>
       <c r="G216" t="inlineStr">
         <is>
@@ -9102,7 +9102,7 @@
         </is>
       </c>
       <c r="F217" t="n">
-        <v>2.142857142857143</v>
+        <v>15</v>
       </c>
       <c r="G217" t="inlineStr">
         <is>
@@ -9142,7 +9142,7 @@
         </is>
       </c>
       <c r="F218" t="n">
-        <v>44.12571428571429</v>
+        <v>308.88</v>
       </c>
       <c r="G218" t="inlineStr">
         <is>
@@ -9182,7 +9182,7 @@
         </is>
       </c>
       <c r="F219" t="n">
-        <v>6.887142857142857</v>
+        <v>48.21</v>
       </c>
       <c r="G219" t="inlineStr">
         <is>
@@ -9222,7 +9222,7 @@
         </is>
       </c>
       <c r="F220" t="n">
-        <v>24.26142857142857</v>
+        <v>169.83</v>
       </c>
       <c r="G220" t="inlineStr">
         <is>
@@ -9262,7 +9262,7 @@
         </is>
       </c>
       <c r="F221" t="n">
-        <v>171.8128571428572</v>
+        <v>1202.69</v>
       </c>
       <c r="G221" t="inlineStr">
         <is>
@@ -9302,7 +9302,7 @@
         </is>
       </c>
       <c r="F222" t="n">
-        <v>1680.244285714286</v>
+        <v>11761.71</v>
       </c>
       <c r="G222" t="inlineStr">
         <is>
@@ -9342,7 +9342,7 @@
         </is>
       </c>
       <c r="F223" t="n">
-        <v>30.29571428571429</v>
+        <v>212.07</v>
       </c>
       <c r="G223" t="inlineStr">
         <is>
@@ -9382,7 +9382,7 @@
         </is>
       </c>
       <c r="F224" t="n">
-        <v>115.7257142857143</v>
+        <v>810.08</v>
       </c>
       <c r="G224" t="inlineStr">
         <is>
@@ -9422,7 +9422,7 @@
         </is>
       </c>
       <c r="F225" t="n">
-        <v>219.5214285714286</v>
+        <v>1536.65</v>
       </c>
       <c r="G225" t="inlineStr">
         <is>
@@ -9462,7 +9462,7 @@
         </is>
       </c>
       <c r="F226" t="n">
-        <v>73.17428571428572</v>
+        <v>512.22</v>
       </c>
       <c r="G226" t="inlineStr">
         <is>
@@ -9502,7 +9502,7 @@
         </is>
       </c>
       <c r="F227" t="n">
-        <v>182.5028571428572</v>
+        <v>1277.52</v>
       </c>
       <c r="G227" t="inlineStr">
         <is>
@@ -9542,7 +9542,7 @@
         </is>
       </c>
       <c r="F228" t="n">
-        <v>13.88285714285714</v>
+        <v>97.18000000000001</v>
       </c>
       <c r="G228" t="inlineStr">
         <is>
@@ -9582,7 +9582,7 @@
         </is>
       </c>
       <c r="F229" t="n">
-        <v>27.93142857142857</v>
+        <v>195.52</v>
       </c>
       <c r="G229" t="inlineStr">
         <is>
@@ -9622,7 +9622,7 @@
         </is>
       </c>
       <c r="F230" t="n">
-        <v>308.1114285714286</v>
+        <v>2156.78</v>
       </c>
       <c r="G230" t="inlineStr">
         <is>
@@ -9662,7 +9662,7 @@
         </is>
       </c>
       <c r="F231" t="n">
-        <v>223.8171428571429</v>
+        <v>1566.72</v>
       </c>
       <c r="G231" t="inlineStr">
         <is>
@@ -9702,7 +9702,7 @@
         </is>
       </c>
       <c r="F232" t="n">
-        <v>31.97428571428571</v>
+        <v>223.82</v>
       </c>
       <c r="G232" t="inlineStr">
         <is>
@@ -9742,7 +9742,7 @@
         </is>
       </c>
       <c r="F233" t="n">
-        <v>440.1128571428571</v>
+        <v>3080.79</v>
       </c>
       <c r="G233" t="inlineStr">
         <is>
@@ -9782,7 +9782,7 @@
         </is>
       </c>
       <c r="F234" t="n">
-        <v>146.7042857142857</v>
+        <v>1026.93</v>
       </c>
       <c r="G234" t="inlineStr">
         <is>
@@ -9822,7 +9822,7 @@
         </is>
       </c>
       <c r="F235" t="n">
-        <v>528.1357142857142</v>
+        <v>3696.95</v>
       </c>
       <c r="G235" t="inlineStr">
         <is>
@@ -9862,7 +9862,7 @@
         </is>
       </c>
       <c r="F236" t="n">
-        <v>33.13142857142857</v>
+        <v>231.92</v>
       </c>
       <c r="G236" t="inlineStr">
         <is>
@@ -9902,7 +9902,7 @@
         </is>
       </c>
       <c r="F237" t="n">
-        <v>11.04428571428572</v>
+        <v>77.31</v>
       </c>
       <c r="G237" t="inlineStr">
         <is>
@@ -9942,7 +9942,7 @@
         </is>
       </c>
       <c r="F238" t="n">
-        <v>0.3628571428571429</v>
+        <v>2.54</v>
       </c>
       <c r="G238" t="inlineStr">
         <is>
@@ -9982,7 +9982,7 @@
         </is>
       </c>
       <c r="F239" t="n">
-        <v>215.9357142857143</v>
+        <v>1511.55</v>
       </c>
       <c r="G239" t="inlineStr">
         <is>
@@ -10022,7 +10022,7 @@
         </is>
       </c>
       <c r="F240" t="n">
-        <v>26.81428571428571</v>
+        <v>187.7</v>
       </c>
       <c r="G240" t="inlineStr">
         <is>
@@ -10062,7 +10062,7 @@
         </is>
       </c>
       <c r="F241" t="n">
-        <v>20.19142857142857</v>
+        <v>141.34</v>
       </c>
       <c r="G241" t="inlineStr">
         <is>
@@ -10102,7 +10102,7 @@
         </is>
       </c>
       <c r="F242" t="n">
-        <v>22.11428571428571</v>
+        <v>154.8</v>
       </c>
       <c r="G242" t="inlineStr">
         <is>
@@ -10142,7 +10142,7 @@
         </is>
       </c>
       <c r="F243" t="n">
-        <v>687.8071428571428</v>
+        <v>4814.65</v>
       </c>
       <c r="G243" t="inlineStr">
         <is>
@@ -10182,7 +10182,7 @@
         </is>
       </c>
       <c r="F244" t="n">
-        <v>0.2828571428571429</v>
+        <v>1.98</v>
       </c>
       <c r="G244" t="inlineStr">
         <is>
@@ -10222,7 +10222,7 @@
         </is>
       </c>
       <c r="F245" t="n">
-        <v>260.5142857142857</v>
+        <v>1823.6</v>
       </c>
       <c r="G245" t="inlineStr">
         <is>
@@ -10262,7 +10262,7 @@
         </is>
       </c>
       <c r="F246" t="n">
-        <v>88.25285714285714</v>
+        <v>617.77</v>
       </c>
       <c r="G246" t="inlineStr">
         <is>
@@ -10302,7 +10302,7 @@
         </is>
       </c>
       <c r="F247" t="n">
-        <v>2.654285714285715</v>
+        <v>18.58</v>
       </c>
       <c r="G247" t="inlineStr">
         <is>
@@ -10342,7 +10342,7 @@
         </is>
       </c>
       <c r="F248" t="n">
-        <v>16.16571428571429</v>
+        <v>113.16</v>
       </c>
       <c r="G248" t="inlineStr">
         <is>
@@ -10382,7 +10382,7 @@
         </is>
       </c>
       <c r="F249" t="n">
-        <v>18.48714285714286</v>
+        <v>129.41</v>
       </c>
       <c r="G249" t="inlineStr">
         <is>
@@ -10422,7 +10422,7 @@
         </is>
       </c>
       <c r="F250" t="n">
-        <v>1856.057142857143</v>
+        <v>12992.4</v>
       </c>
       <c r="G250" t="inlineStr">
         <is>
@@ -10462,7 +10462,7 @@
         </is>
       </c>
       <c r="F251" t="n">
-        <v>61.90428571428571</v>
+        <v>433.33</v>
       </c>
       <c r="G251" t="inlineStr">
         <is>
@@ -10502,7 +10502,7 @@
         </is>
       </c>
       <c r="F252" t="n">
-        <v>2.571428571428571</v>
+        <v>18</v>
       </c>
       <c r="G252" t="inlineStr">
         <is>
@@ -10542,7 +10542,7 @@
         </is>
       </c>
       <c r="F253" t="n">
-        <v>3.871428571428571</v>
+        <v>27.1</v>
       </c>
       <c r="G253" t="inlineStr">
         <is>
@@ -10582,7 +10582,7 @@
         </is>
       </c>
       <c r="F254" t="n">
-        <v>5.367142857142857</v>
+        <v>37.57</v>
       </c>
       <c r="G254" t="inlineStr">
         <is>
@@ -10622,7 +10622,7 @@
         </is>
       </c>
       <c r="F255" t="n">
-        <v>33.13142857142857</v>
+        <v>231.92</v>
       </c>
       <c r="G255" t="inlineStr">
         <is>
@@ -10662,7 +10662,7 @@
         </is>
       </c>
       <c r="F256" t="n">
-        <v>11.04428571428572</v>
+        <v>77.31</v>
       </c>
       <c r="G256" t="inlineStr">
         <is>
@@ -10702,7 +10702,7 @@
         </is>
       </c>
       <c r="F257" t="n">
-        <v>673.9057142857142</v>
+        <v>4717.34</v>
       </c>
       <c r="G257" t="inlineStr">
         <is>
@@ -10742,7 +10742,7 @@
         </is>
       </c>
       <c r="F258" t="n">
-        <v>711.5314285714287</v>
+        <v>4980.72</v>
       </c>
       <c r="G258" t="inlineStr">
         <is>
@@ -10782,7 +10782,7 @@
         </is>
       </c>
       <c r="F259" t="n">
-        <v>13.37571428571428</v>
+        <v>93.63</v>
       </c>
       <c r="G259" t="inlineStr">
         <is>
@@ -10822,7 +10822,7 @@
         </is>
       </c>
       <c r="F260" t="n">
-        <v>212.3142857142857</v>
+        <v>1486.2</v>
       </c>
       <c r="G260" t="inlineStr">
         <is>
@@ -10862,7 +10862,7 @@
         </is>
       </c>
       <c r="F261" t="n">
-        <v>2.597142857142857</v>
+        <v>18.18</v>
       </c>
       <c r="G261" t="inlineStr">
         <is>
@@ -10902,7 +10902,7 @@
         </is>
       </c>
       <c r="F262" t="n">
-        <v>66.95285714285714</v>
+        <v>468.67</v>
       </c>
       <c r="G262" t="inlineStr">
         <is>
@@ -10942,7 +10942,7 @@
         </is>
       </c>
       <c r="F263" t="n">
-        <v>0.1971428571428571</v>
+        <v>1.38</v>
       </c>
       <c r="G263" t="inlineStr">
         <is>
@@ -10982,7 +10982,7 @@
         </is>
       </c>
       <c r="F264" t="n">
-        <v>92.65428571428572</v>
+        <v>648.5799999999999</v>
       </c>
       <c r="G264" t="inlineStr">
         <is>
@@ -11022,7 +11022,7 @@
         </is>
       </c>
       <c r="F265" t="n">
-        <v>284.6671428571429</v>
+        <v>1992.67</v>
       </c>
       <c r="G265" t="inlineStr">
         <is>
@@ -11062,7 +11062,7 @@
         </is>
       </c>
       <c r="F266" t="n">
-        <v>0.1542857142857143</v>
+        <v>1.08</v>
       </c>
       <c r="G266" t="inlineStr">
         <is>
@@ -11102,7 +11102,7 @@
         </is>
       </c>
       <c r="F267" t="n">
-        <v>6.685714285714285</v>
+        <v>46.8</v>
       </c>
       <c r="G267" t="inlineStr">
         <is>
@@ -11142,7 +11142,7 @@
         </is>
       </c>
       <c r="F268" t="n">
-        <v>27.09142857142857</v>
+        <v>189.64</v>
       </c>
       <c r="G268" t="inlineStr">
         <is>
@@ -11182,7 +11182,7 @@
         </is>
       </c>
       <c r="F269" t="n">
-        <v>3.818571428571429</v>
+        <v>26.73</v>
       </c>
       <c r="G269" t="inlineStr">
         <is>
@@ -11222,7 +11222,7 @@
         </is>
       </c>
       <c r="F270" t="n">
-        <v>19.57428571428571</v>
+        <v>137.02</v>
       </c>
       <c r="G270" t="inlineStr">
         <is>
@@ -11262,7 +11262,7 @@
         </is>
       </c>
       <c r="F271" t="n">
-        <v>7.037142857142856</v>
+        <v>49.26</v>
       </c>
       <c r="G271" t="inlineStr">
         <is>
@@ -11302,7 +11302,7 @@
         </is>
       </c>
       <c r="F272" t="n">
-        <v>0.8571428571428571</v>
+        <v>6</v>
       </c>
       <c r="G272" t="inlineStr">
         <is>
@@ -11342,7 +11342,7 @@
         </is>
       </c>
       <c r="F273" t="n">
-        <v>80.2342857142857</v>
+        <v>561.64</v>
       </c>
       <c r="G273" t="inlineStr">
         <is>

</xml_diff>